<commit_message>
Mise à jour des fichiers de données
</commit_message>
<xml_diff>
--- a/data/ecological_data.xlsx
+++ b/data/ecological_data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="162">
   <si>
     <t xml:space="preserve">Resampled, Randomized Data</t>
   </si>
@@ -1737,6 +1737,9 @@
       <t xml:space="preserve">ee fig. S5 for additional details</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
 </sst>
 </file>
 
@@ -1757,7 +1760,7 @@
     <numFmt numFmtId="175" formatCode="[&lt;0.005]0.00E+00;0.000"/>
     <numFmt numFmtId="176" formatCode="[&lt;0.005]0.00E+00\ǂ;0.000\ǂ"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1844,13 +1847,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2023,7 +2019,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="144">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2544,8 +2540,60 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -10309,7 +10357,7 @@
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
   </cols>
@@ -20640,7 +20688,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.85"/>
@@ -26172,7 +26220,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="9.83"/>
@@ -27545,7 +27593,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.65"/>
@@ -28572,7 +28620,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.16"/>
@@ -28801,1897 +28849,1798 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="979" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="130" width="27.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="977" min="2" style="130" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="978" style="130" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="131" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="130" t="s">
+      <c r="B1" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="133" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="133" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="133" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="134" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="133"/>
+      <c r="J1" s="134" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="135" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="135" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="130" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="27" t="n">
+      <c r="B3" s="136" t="n">
         <v>2.67533</v>
       </c>
-      <c r="C3" s="28" t="n">
+      <c r="C3" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D4/$B3</f>
         <v>1.4390748057249</v>
       </c>
-      <c r="D3" s="30" t="n">
+      <c r="D3" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J4/$B3</f>
         <v>0.5868434922047</v>
       </c>
-      <c r="E3" s="28" t="n">
+      <c r="E3" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P4/$B3</f>
         <v>0.590581348842946</v>
       </c>
-      <c r="F3" s="30" t="n">
+      <c r="F3" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V4/$B3</f>
         <v>4.99003861205907</v>
       </c>
-      <c r="G3" s="28" t="n">
+      <c r="G3" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB4/$B3</f>
         <v>2.67630535298449</v>
       </c>
-      <c r="H3" s="33" t="n">
+      <c r="H3" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH4/$B3</f>
         <v>242.026217326461</v>
       </c>
-      <c r="I3" s="33" t="n">
+      <c r="I3" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI4/$B3</f>
         <v>156.690950275293</v>
       </c>
-      <c r="J3" s="33" t="n">
+      <c r="J3" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN4/$B3</f>
         <v>12479.0586581842</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="27" t="n">
+      <c r="B4" s="136" t="n">
         <v>4.5225</v>
       </c>
-      <c r="C4" s="28" t="n">
+      <c r="C4" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D5/$B4</f>
         <v>0.650082918739635</v>
       </c>
-      <c r="D4" s="30" t="n">
+      <c r="D4" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J5/$B4</f>
         <v>0.375898286346048</v>
       </c>
-      <c r="E4" s="28" t="n">
+      <c r="E4" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P5/$B4</f>
         <v>0.371475953565506</v>
       </c>
-      <c r="F4" s="30" t="n">
+      <c r="F4" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V5/$B4</f>
         <v>2.58264234383637</v>
       </c>
-      <c r="G4" s="28" t="n">
+      <c r="G4" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB5/$B4</f>
         <v>0.89110005527916</v>
       </c>
-      <c r="H4" s="33" t="n">
+      <c r="H4" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH5/$B4</f>
         <v>47.6948590381426</v>
       </c>
-      <c r="I4" s="33" t="n">
+      <c r="I4" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI5/$B4</f>
         <v>9.70702045328911</v>
       </c>
-      <c r="J4" s="33" t="n">
+      <c r="J4" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN5/$B4</f>
         <v>2402.05638474295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="35" t="n">
+      <c r="B5" s="140" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="n">
+      <c r="C5" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D6/$B5</f>
         <v>0.222</v>
       </c>
-      <c r="D5" s="30" t="n">
+      <c r="D5" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J6/$B5</f>
         <v>0.236</v>
       </c>
-      <c r="E5" s="28" t="n">
+      <c r="E5" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P6/$B5</f>
         <v>0.236</v>
       </c>
-      <c r="F5" s="30" t="n">
+      <c r="F5" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V6/$B5</f>
         <v>1.318</v>
       </c>
-      <c r="G5" s="28" t="n">
+      <c r="G5" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB6/$B5</f>
         <v>0.466</v>
       </c>
-      <c r="H5" s="33" t="n">
+      <c r="H5" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH6/$B5</f>
         <v>3.42</v>
       </c>
-      <c r="I5" s="33" t="n">
+      <c r="I5" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI6/$B5</f>
         <v>1.4</v>
       </c>
-      <c r="J5" s="33" t="n">
+      <c r="J5" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN6/$B5</f>
         <v>139.28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="27" t="n">
+      <c r="B6" s="136" t="n">
         <v>2.623</v>
       </c>
-      <c r="C6" s="28" t="n">
+      <c r="C6" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D7/$B6</f>
         <v>2.89744567289363</v>
       </c>
-      <c r="D6" s="30" t="n">
+      <c r="D6" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J7/$B6</f>
         <v>0.945482272207396</v>
       </c>
-      <c r="E6" s="28" t="n">
+      <c r="E6" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P7/$B6</f>
         <v>0.941669843690431</v>
       </c>
-      <c r="F6" s="30" t="n">
+      <c r="F6" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V7/$B6</f>
         <v>4.07167365611895</v>
       </c>
-      <c r="G6" s="28" t="n">
+      <c r="G6" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB7/$B6</f>
         <v>4.28135722455204</v>
       </c>
-      <c r="H6" s="33" t="n">
+      <c r="H6" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH7/$B6</f>
         <v>183.911551658406</v>
       </c>
-      <c r="I6" s="33" t="n">
+      <c r="I6" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI7/$B6</f>
         <v>255.547083492184</v>
       </c>
-      <c r="J6" s="33" t="n">
+      <c r="J6" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN7/$B6</f>
         <v>7162.10446054136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="27" t="n">
+      <c r="B7" s="136" t="n">
         <v>3.686</v>
       </c>
-      <c r="C7" s="28" t="n">
+      <c r="C7" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D8/$B7</f>
         <v>0.759631036353771</v>
       </c>
-      <c r="D7" s="30" t="n">
+      <c r="D7" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J8/$B7</f>
         <v>1.2072707542051</v>
       </c>
-      <c r="E7" s="28" t="n">
+      <c r="E7" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P8/$B7</f>
         <v>1.03364080303852</v>
       </c>
-      <c r="F7" s="30" t="n">
+      <c r="F7" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V8/$B7</f>
         <v>7.37655995659251</v>
       </c>
-      <c r="G7" s="28" t="n">
+      <c r="G7" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB8/$B7</f>
         <v>9.51437873033098</v>
       </c>
-      <c r="H7" s="33" t="n">
+      <c r="H7" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH8/$B7</f>
         <v>609.983722192078</v>
       </c>
-      <c r="I7" s="33" t="n">
+      <c r="I7" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI8/$B7</f>
         <v>427.265328269126</v>
       </c>
-      <c r="J7" s="33" t="n">
+      <c r="J7" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN8/$B7</f>
         <v>13449.8914812805</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="27" t="n">
+      <c r="B8" s="136" t="n">
         <v>0.732</v>
       </c>
-      <c r="C8" s="28" t="n">
+      <c r="C8" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D9/$B8</f>
         <v>1.20218579234973</v>
       </c>
-      <c r="D8" s="30" t="n">
+      <c r="D8" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J9/$B8</f>
         <v>0.628415300546448</v>
       </c>
-      <c r="E8" s="28" t="n">
+      <c r="E8" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P9/$B8</f>
         <v>0.614754098360656</v>
       </c>
-      <c r="F8" s="30" t="n">
+      <c r="F8" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V9/$B8</f>
         <v>5.28688524590164</v>
       </c>
-      <c r="G8" s="28" t="n">
+      <c r="G8" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB9/$B8</f>
         <v>4.75409836065574</v>
       </c>
-      <c r="H8" s="33" t="n">
+      <c r="H8" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH9/$B8</f>
         <v>80.7377049180328</v>
       </c>
-      <c r="I8" s="33" t="n">
+      <c r="I8" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI9/$B8</f>
         <v>3.55191256830601</v>
       </c>
-      <c r="J8" s="33" t="n">
+      <c r="J8" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN9/$B8</f>
         <v>3762.56830601093</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="27" t="n">
+      <c r="B9" s="136" t="n">
         <v>0.974</v>
       </c>
-      <c r="C9" s="28" t="n">
+      <c r="C9" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D10/$B9</f>
         <v>1.85831622176591</v>
       </c>
-      <c r="D9" s="30" t="n">
+      <c r="D9" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J10/$B9</f>
         <v>1.35523613963039</v>
       </c>
-      <c r="E9" s="28" t="n">
+      <c r="E9" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P10/$B9</f>
         <v>1.3347022587269</v>
       </c>
-      <c r="F9" s="30" t="n">
+      <c r="F9" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V10/$B9</f>
         <v>3.51129363449692</v>
       </c>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB10/$B9</f>
         <v>0.708418891170431</v>
       </c>
-      <c r="H9" s="33" t="n">
+      <c r="H9" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH10/$B9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="33" t="n">
+      <c r="I9" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI10/$B9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="33" t="n">
+      <c r="J9" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN10/$B9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="28" t="n">
+      <c r="B10" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D11</f>
         <v>2.04</v>
       </c>
-      <c r="D10" s="30" t="n">
+      <c r="D10" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J11</f>
         <v>3.2</v>
       </c>
-      <c r="E10" s="28" t="n">
+      <c r="E10" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P11</f>
         <v>3.16</v>
       </c>
-      <c r="F10" s="30" t="n">
+      <c r="F10" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V11</f>
         <v>18.02</v>
       </c>
-      <c r="G10" s="28" t="n">
+      <c r="G10" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB11</f>
         <v>16.92</v>
       </c>
-      <c r="H10" s="33" t="n">
+      <c r="H10" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH11</f>
         <v>620.1</v>
       </c>
-      <c r="I10" s="33" t="n">
+      <c r="I10" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI11</f>
         <v>8.1</v>
       </c>
-      <c r="J10" s="33" t="n">
+      <c r="J10" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN11</f>
         <v>16438.6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="28" t="n">
+      <c r="B11" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D12</f>
         <v>1.83</v>
       </c>
-      <c r="D11" s="30" t="n">
+      <c r="D11" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J12</f>
         <v>1.81</v>
       </c>
-      <c r="E11" s="28" t="n">
+      <c r="E11" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P12</f>
         <v>1.8</v>
       </c>
-      <c r="F11" s="30" t="n">
+      <c r="F11" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V12</f>
         <v>12.62</v>
       </c>
-      <c r="G11" s="28" t="n">
+      <c r="G11" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB12</f>
         <v>5.41</v>
       </c>
-      <c r="H11" s="33" t="n">
+      <c r="H11" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH12</f>
         <v>217.7</v>
       </c>
-      <c r="I11" s="33" t="n">
+      <c r="I11" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI12</f>
         <v>12.1</v>
       </c>
-      <c r="J11" s="33" t="n">
+      <c r="J11" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN12</f>
         <v>9493.3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="27" t="n">
+      <c r="B12" s="136" t="n">
         <v>2.141</v>
       </c>
-      <c r="C12" s="28" t="n">
+      <c r="C12" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D13/$B12</f>
         <v>7.27230266230733</v>
       </c>
-      <c r="D12" s="30" t="n">
+      <c r="D12" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J13/$B12</f>
         <v>0.83605791686128</v>
       </c>
-      <c r="E12" s="28" t="n">
+      <c r="E12" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P13/$B12</f>
         <v>0.83605791686128</v>
       </c>
-      <c r="F12" s="30" t="n">
+      <c r="F12" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V13/$B12</f>
         <v>10.3082671648762</v>
       </c>
-      <c r="G12" s="28" t="n">
+      <c r="G12" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB13/$B12</f>
         <v>7.97758056982718</v>
       </c>
-      <c r="H12" s="33" t="n">
+      <c r="H12" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH13/$B12</f>
         <v>203.503035964503</v>
       </c>
-      <c r="I12" s="33" t="n">
+      <c r="I12" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI13/$B12</f>
         <v>0</v>
       </c>
-      <c r="J12" s="33" t="n">
+      <c r="J12" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN13/$B12</f>
         <v>10498.552078468</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="27" t="n">
+      <c r="B13" s="136" t="n">
         <v>2.222</v>
       </c>
-      <c r="C13" s="28" t="n">
+      <c r="C13" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D14/$B13</f>
         <v>3.35733573357336</v>
       </c>
-      <c r="D13" s="30" t="n">
+      <c r="D13" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J14/$B13</f>
         <v>0.441044104410441</v>
       </c>
-      <c r="E13" s="28" t="n">
+      <c r="E13" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P14/$B13</f>
         <v>0.436543654365437</v>
       </c>
-      <c r="F13" s="30" t="n">
+      <c r="F13" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V14/$B13</f>
         <v>3.82088208820882</v>
       </c>
-      <c r="G13" s="28" t="n">
+      <c r="G13" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB14/$B13</f>
         <v>3.38433843384338</v>
       </c>
-      <c r="H13" s="33" t="n">
+      <c r="H13" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH14/$B13</f>
         <v>178.487848784879</v>
       </c>
-      <c r="I13" s="33" t="n">
+      <c r="I13" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI14/$B13</f>
         <v>0</v>
       </c>
-      <c r="J13" s="33" t="n">
+      <c r="J13" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN14/$B13</f>
         <v>12577.9477947795</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="27" t="n">
+      <c r="B14" s="136" t="n">
         <v>1.633</v>
       </c>
-      <c r="C14" s="28" t="n">
+      <c r="C14" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D15/$B14</f>
         <v>7.93631353337416</v>
       </c>
-      <c r="D14" s="30" t="n">
+      <c r="D14" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J15/$B14</f>
         <v>0.263319044703001</v>
       </c>
-      <c r="E14" s="28" t="n">
+      <c r="E14" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P15/$B14</f>
         <v>0.226576852418861</v>
       </c>
-      <c r="F14" s="30" t="n">
+      <c r="F14" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V15/$B14</f>
         <v>27.6484996938151</v>
       </c>
-      <c r="G14" s="28" t="n">
+      <c r="G14" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB15/$B14</f>
         <v>11.7268830373546</v>
       </c>
-      <c r="H14" s="33" t="n">
+      <c r="H14" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH15/$B14</f>
         <v>2531.41457440294</v>
       </c>
-      <c r="I14" s="33" t="n">
+      <c r="I14" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI15/$B14</f>
         <v>1116.53398652786</v>
       </c>
-      <c r="J14" s="33" t="n">
+      <c r="J14" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN15/$B14</f>
         <v>140777.587262707</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="27" t="n">
+      <c r="B15" s="136" t="n">
         <v>2.618</v>
       </c>
-      <c r="C15" s="28" t="n">
+      <c r="C15" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D16/$B15</f>
         <v>3.47975553857907</v>
       </c>
-      <c r="D15" s="30" t="n">
+      <c r="D15" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J16/$B15</f>
         <v>1.23376623376623</v>
       </c>
-      <c r="E15" s="28" t="n">
+      <c r="E15" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P16/$B15</f>
         <v>1.21466768525592</v>
       </c>
-      <c r="F15" s="30" t="n">
+      <c r="F15" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V16/$B15</f>
         <v>8.6401833460657</v>
       </c>
-      <c r="G15" s="28" t="n">
+      <c r="G15" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB16/$B15</f>
         <v>5.40106951871658</v>
       </c>
-      <c r="H15" s="33" t="n">
+      <c r="H15" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH16/$B15</f>
         <v>707.524828113063</v>
       </c>
-      <c r="I15" s="33" t="n">
+      <c r="I15" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI16/$B15</f>
         <v>343.850267379679</v>
       </c>
-      <c r="J15" s="33" t="n">
+      <c r="J15" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN16/$B15</f>
         <v>23605.0038197097</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="130" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="28" t="n">
+      <c r="B16" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D17</f>
         <v>0.66</v>
       </c>
-      <c r="D16" s="30" t="n">
+      <c r="D16" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J17</f>
         <v>0.98</v>
       </c>
-      <c r="E16" s="28" t="n">
+      <c r="E16" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P17</f>
         <v>0.97</v>
       </c>
-      <c r="F16" s="30" t="n">
+      <c r="F16" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V17</f>
         <v>2.6</v>
       </c>
-      <c r="G16" s="28" t="n">
+      <c r="G16" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB17</f>
         <v>1.06</v>
       </c>
-      <c r="H16" s="33" t="n">
+      <c r="H16" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH17</f>
         <v>27.8</v>
       </c>
-      <c r="I16" s="33" t="n">
+      <c r="I16" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI17</f>
         <v>1.3</v>
       </c>
-      <c r="J16" s="33" t="n">
+      <c r="J16" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN17</f>
         <v>955.6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="40" t="n">
+      <c r="B17" s="142" t="n">
         <v>1.6</v>
       </c>
-      <c r="C17" s="28" t="n">
+      <c r="C17" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D18/$B17</f>
         <v>2.2</v>
       </c>
-      <c r="D17" s="30" t="n">
+      <c r="D17" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J18/$B17</f>
         <v>1.975</v>
       </c>
-      <c r="E17" s="28" t="n">
+      <c r="E17" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P18/$B17</f>
         <v>1.9625</v>
       </c>
-      <c r="F17" s="30" t="n">
+      <c r="F17" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V18/$B17</f>
         <v>4.1875</v>
       </c>
-      <c r="G17" s="28" t="n">
+      <c r="G17" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB18/$B17</f>
         <v>3.85</v>
       </c>
-      <c r="H17" s="33" t="n">
+      <c r="H17" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH18/$B17</f>
         <v>92.875</v>
       </c>
-      <c r="I17" s="33" t="n">
+      <c r="I17" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI18/$B17</f>
         <v>4.125</v>
       </c>
-      <c r="J17" s="33" t="n">
+      <c r="J17" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN18/$B17</f>
         <v>3195.75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="28" t="n">
+      <c r="B18" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D19</f>
         <v>10.52</v>
       </c>
-      <c r="D18" s="30" t="n">
+      <c r="D18" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J19</f>
         <v>6.32</v>
       </c>
-      <c r="E18" s="28" t="n">
+      <c r="E18" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P19</f>
         <v>6.15</v>
       </c>
-      <c r="F18" s="30" t="n">
+      <c r="F18" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V19</f>
         <v>15.67</v>
       </c>
-      <c r="G18" s="28" t="n">
+      <c r="G18" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB19</f>
         <v>11.69</v>
       </c>
-      <c r="H18" s="33" t="n">
+      <c r="H18" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH19</f>
         <v>414.6</v>
       </c>
-      <c r="I18" s="33" t="n">
+      <c r="I18" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI19</f>
         <v>1.6</v>
       </c>
-      <c r="J18" s="33" t="n">
+      <c r="J18" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN19</f>
         <v>14888.2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="28" t="n">
+      <c r="B19" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D20</f>
         <v>2.42</v>
       </c>
-      <c r="D19" s="30" t="n">
+      <c r="D19" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J20</f>
         <v>7.32</v>
       </c>
-      <c r="E19" s="28" t="n">
+      <c r="E19" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P20</f>
         <v>7.16</v>
       </c>
-      <c r="F19" s="30" t="n">
+      <c r="F19" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V20</f>
         <v>17.52</v>
       </c>
-      <c r="G19" s="28" t="n">
+      <c r="G19" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB20</f>
         <v>10.67</v>
       </c>
-      <c r="H19" s="33" t="n">
+      <c r="H19" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH20</f>
         <v>6.4</v>
       </c>
-      <c r="I19" s="33" t="n">
+      <c r="I19" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI20</f>
         <v>6.4</v>
       </c>
-      <c r="J19" s="33" t="n">
+      <c r="J19" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN20</f>
         <v>36.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="28" t="n">
+      <c r="B20" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D21</f>
         <v>17.66</v>
       </c>
-      <c r="D20" s="30" t="n">
+      <c r="D20" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J21</f>
         <v>3.6</v>
       </c>
-      <c r="E20" s="28" t="n">
+      <c r="E20" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P21</f>
         <v>3.59</v>
       </c>
-      <c r="F20" s="30" t="n">
+      <c r="F20" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V21</f>
         <v>27.96</v>
       </c>
-      <c r="G20" s="28" t="n">
+      <c r="G20" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB21</f>
         <v>50.66</v>
       </c>
-      <c r="H20" s="33" t="n">
+      <c r="H20" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH21</f>
         <v>1007.9</v>
       </c>
-      <c r="I20" s="33" t="n">
+      <c r="I20" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI21</f>
         <v>10.2</v>
       </c>
-      <c r="J20" s="33" t="n">
+      <c r="J20" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN21</f>
         <v>36369.4</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="28" t="n">
+      <c r="B21" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D22</f>
         <v>10.63</v>
       </c>
-      <c r="D21" s="30" t="n">
+      <c r="D21" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J22</f>
         <v>3.77</v>
       </c>
-      <c r="E21" s="28" t="n">
+      <c r="E21" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P22</f>
         <v>3.76</v>
       </c>
-      <c r="F21" s="30" t="n">
+      <c r="F21" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V22</f>
         <v>28.51</v>
       </c>
-      <c r="G21" s="28" t="n">
+      <c r="G21" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB22</f>
         <v>19.19</v>
       </c>
-      <c r="H21" s="33" t="n">
+      <c r="H21" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH22</f>
         <v>237.7</v>
       </c>
-      <c r="I21" s="33" t="n">
+      <c r="I21" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI22</f>
         <v>1.4</v>
       </c>
-      <c r="J21" s="33" t="n">
+      <c r="J21" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN22</f>
         <v>10593.7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="28" t="n">
+      <c r="B22" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D23</f>
         <v>26.31</v>
       </c>
-      <c r="D22" s="30" t="n">
+      <c r="D22" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J23</f>
         <v>5.42</v>
       </c>
-      <c r="E22" s="28" t="n">
+      <c r="E22" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P23</f>
         <v>5.25</v>
       </c>
-      <c r="F22" s="30" t="n">
+      <c r="F22" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V23</f>
         <v>37.58</v>
       </c>
-      <c r="G22" s="28" t="n">
+      <c r="G22" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB23</f>
         <v>37.26</v>
       </c>
-      <c r="H22" s="33" t="n">
+      <c r="H22" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH23</f>
         <v>2141.8</v>
       </c>
-      <c r="I22" s="33" t="n">
+      <c r="I22" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI23</f>
         <v>317.9</v>
       </c>
-      <c r="J22" s="33" t="n">
+      <c r="J22" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN23</f>
         <v>177480.2</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="28" t="n">
+      <c r="B23" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D24</f>
         <v>0.8</v>
       </c>
-      <c r="D23" s="30" t="n">
+      <c r="D23" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J24</f>
         <v>2.09</v>
       </c>
-      <c r="E23" s="28" t="n">
+      <c r="E23" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P24</f>
         <v>2.01</v>
       </c>
-      <c r="F23" s="30" t="n">
+      <c r="F23" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V24</f>
         <v>17.21</v>
       </c>
-      <c r="G23" s="28" t="n">
+      <c r="G23" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB24</f>
         <v>7.51</v>
       </c>
-      <c r="H23" s="33" t="n">
+      <c r="H23" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH24</f>
         <v>369.8</v>
       </c>
-      <c r="I23" s="33" t="n">
+      <c r="I23" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI24</f>
         <v>77</v>
       </c>
-      <c r="J23" s="33" t="n">
+      <c r="J23" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN24</f>
         <v>5335.7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="28" t="n">
+      <c r="B24" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D25</f>
         <v>0.39</v>
       </c>
-      <c r="D24" s="30" t="n">
+      <c r="D24" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J25</f>
         <v>0.5</v>
       </c>
-      <c r="E24" s="28" t="n">
+      <c r="E24" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P25</f>
         <v>0.5</v>
       </c>
-      <c r="F24" s="30" t="n">
+      <c r="F24" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V25</f>
         <v>3.63</v>
       </c>
-      <c r="G24" s="28" t="n">
+      <c r="G24" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB25</f>
         <v>3.24</v>
       </c>
-      <c r="H24" s="33" t="n">
+      <c r="H24" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH25</f>
         <v>14.3</v>
       </c>
-      <c r="I24" s="33" t="n">
+      <c r="I24" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI25</f>
         <v>1.9</v>
       </c>
-      <c r="J24" s="33" t="n">
+      <c r="J24" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN25</f>
         <v>932</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="28" t="n">
+      <c r="B25" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D26</f>
         <v>0.33</v>
       </c>
-      <c r="D25" s="30" t="n">
+      <c r="D25" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J26</f>
         <v>0.43</v>
       </c>
-      <c r="E25" s="28" t="n">
+      <c r="E25" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P26</f>
         <v>0.43</v>
       </c>
-      <c r="F25" s="30" t="n">
+      <c r="F25" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V26</f>
         <v>2.9</v>
       </c>
-      <c r="G25" s="28" t="n">
+      <c r="G25" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB26</f>
         <v>1.61</v>
       </c>
-      <c r="H25" s="33" t="n">
+      <c r="H25" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH26</f>
         <v>28.4</v>
       </c>
-      <c r="I25" s="33" t="n">
+      <c r="I25" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI26</f>
         <v>9.9</v>
       </c>
-      <c r="J25" s="33" t="n">
+      <c r="J25" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN26</f>
         <v>929.2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="28" t="n">
+      <c r="B26" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D27</f>
         <v>0.55</v>
       </c>
-      <c r="D26" s="30" t="n">
+      <c r="D26" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J27</f>
         <v>0.51</v>
       </c>
-      <c r="E26" s="28" t="n">
+      <c r="E26" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P27</f>
         <v>0.51</v>
       </c>
-      <c r="F26" s="30" t="n">
+      <c r="F26" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V27</f>
         <v>8.21</v>
       </c>
-      <c r="G26" s="28" t="n">
+      <c r="G26" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB27</f>
         <v>5.01</v>
       </c>
-      <c r="H26" s="33" t="n">
+      <c r="H26" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH27</f>
         <v>119.4</v>
       </c>
-      <c r="I26" s="33" t="n">
+      <c r="I26" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI27</f>
         <v>54.5</v>
       </c>
-      <c r="J26" s="33" t="n">
+      <c r="J26" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN27</f>
         <v>8455.1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="28" t="n">
+      <c r="B27" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D28</f>
         <v>0.38</v>
       </c>
-      <c r="D27" s="30" t="n">
+      <c r="D27" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J28</f>
         <v>0.53</v>
       </c>
-      <c r="E27" s="28" t="n">
+      <c r="E27" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P28</f>
         <v>0.53</v>
       </c>
-      <c r="F27" s="30" t="n">
+      <c r="F27" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V28</f>
         <v>6.41</v>
       </c>
-      <c r="G27" s="28" t="n">
+      <c r="G27" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB28</f>
         <v>2.27</v>
       </c>
-      <c r="H27" s="33" t="n">
+      <c r="H27" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH28</f>
         <v>102.5</v>
       </c>
-      <c r="I27" s="33" t="n">
+      <c r="I27" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI28</f>
         <v>81.3</v>
       </c>
-      <c r="J27" s="33" t="n">
+      <c r="J27" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN28</f>
         <v>4911.4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="28" t="n">
+      <c r="B28" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D29</f>
         <v>0.86</v>
       </c>
-      <c r="D28" s="30" t="n">
+      <c r="D28" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J29</f>
         <v>0.39</v>
       </c>
-      <c r="E28" s="28" t="n">
+      <c r="E28" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P29</f>
         <v>0.37</v>
       </c>
-      <c r="F28" s="30" t="n">
+      <c r="F28" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V29</f>
         <v>4.04</v>
       </c>
-      <c r="G28" s="28" t="n">
+      <c r="G28" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB29</f>
         <v>2.24</v>
       </c>
-      <c r="H28" s="33" t="n">
+      <c r="H28" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH29</f>
         <v>82.7</v>
       </c>
-      <c r="I28" s="33" t="n">
+      <c r="I28" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI29</f>
         <v>37.4</v>
       </c>
-      <c r="J28" s="33" t="n">
+      <c r="J28" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN29</f>
         <v>4662.7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="28" t="n">
+      <c r="B29" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D30</f>
         <v>1.93</v>
       </c>
-      <c r="D29" s="30" t="n">
+      <c r="D29" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J30</f>
         <v>0.86</v>
       </c>
-      <c r="E29" s="28" t="n">
+      <c r="E29" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P30</f>
         <v>0.86</v>
       </c>
-      <c r="F29" s="30" t="n">
+      <c r="F29" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V30</f>
         <v>6.35</v>
       </c>
-      <c r="G29" s="28" t="n">
+      <c r="G29" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB30</f>
         <v>3.29</v>
       </c>
-      <c r="H29" s="33" t="n">
+      <c r="H29" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH30</f>
         <v>114.5</v>
       </c>
-      <c r="I29" s="33" t="n">
+      <c r="I29" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI30</f>
         <v>1</v>
       </c>
-      <c r="J29" s="33" t="n">
+      <c r="J29" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN30</f>
         <v>661.9</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="28" t="n">
+      <c r="B30" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C30" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D31</f>
         <v>0.63</v>
       </c>
-      <c r="D30" s="30" t="n">
+      <c r="D30" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J31</f>
         <v>0.43</v>
       </c>
-      <c r="E30" s="28" t="n">
+      <c r="E30" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P31</f>
         <v>0.42</v>
       </c>
-      <c r="F30" s="30" t="n">
+      <c r="F30" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V31</f>
         <v>3.52</v>
       </c>
-      <c r="G30" s="28" t="n">
+      <c r="G30" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB31</f>
         <v>1.45</v>
       </c>
-      <c r="H30" s="33" t="n">
+      <c r="H30" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH31</f>
         <v>180.1</v>
       </c>
-      <c r="I30" s="33" t="n">
+      <c r="I30" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI31</f>
         <v>114.5</v>
       </c>
-      <c r="J30" s="33" t="n">
+      <c r="J30" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN31</f>
         <v>12948.6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="28" t="n">
+      <c r="B31" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D32</f>
         <v>2.41</v>
       </c>
-      <c r="D31" s="30" t="n">
+      <c r="D31" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J32</f>
         <v>1.53</v>
       </c>
-      <c r="E31" s="28" t="n">
+      <c r="E31" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P32</f>
         <v>1.52</v>
       </c>
-      <c r="F31" s="30" t="n">
+      <c r="F31" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V32</f>
         <v>12.29</v>
       </c>
-      <c r="G31" s="28" t="n">
+      <c r="G31" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB32</f>
         <v>6.12</v>
       </c>
-      <c r="H31" s="33" t="n">
+      <c r="H31" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH32</f>
         <v>419.6</v>
       </c>
-      <c r="I31" s="33" t="n">
+      <c r="I31" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI32</f>
         <v>403.5</v>
       </c>
-      <c r="J31" s="33" t="n">
+      <c r="J31" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN32</f>
         <v>21162.1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="35" t="n">
+      <c r="B32" s="140" t="n">
         <v>12.5</v>
       </c>
-      <c r="C32" s="28" t="n">
+      <c r="C32" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D33/$B32</f>
         <v>0.1424</v>
       </c>
-      <c r="D32" s="30" t="n">
+      <c r="D32" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J33/$B32</f>
         <v>0.1432</v>
       </c>
-      <c r="E32" s="28" t="n">
+      <c r="E32" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P33/$B32</f>
         <v>0.1408</v>
       </c>
-      <c r="F32" s="30" t="n">
+      <c r="F32" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V33/$B32</f>
         <v>1.0208</v>
       </c>
-      <c r="G32" s="28" t="n">
+      <c r="G32" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB33/$B32</f>
         <v>0.3656</v>
       </c>
-      <c r="H32" s="33" t="n">
+      <c r="H32" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH33/$B32</f>
         <v>6.312</v>
       </c>
-      <c r="I32" s="33" t="n">
+      <c r="I32" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI33/$B32</f>
         <v>0.36</v>
       </c>
-      <c r="J32" s="33" t="n">
+      <c r="J32" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN33/$B32</f>
         <v>91.944</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="28" t="n">
+      <c r="B33" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D34</f>
         <v>0.89</v>
       </c>
-      <c r="D33" s="30" t="n">
+      <c r="D33" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J34</f>
         <v>1.05</v>
       </c>
-      <c r="E33" s="28" t="n">
+      <c r="E33" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P34</f>
         <v>1.06</v>
       </c>
-      <c r="F33" s="30" t="n">
+      <c r="F33" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V34</f>
         <v>5.78</v>
       </c>
-      <c r="G33" s="28" t="n">
+      <c r="G33" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB34</f>
         <v>2.43</v>
       </c>
-      <c r="H33" s="33" t="n">
+      <c r="H33" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH34</f>
         <v>153.5</v>
       </c>
-      <c r="I33" s="33" t="n">
+      <c r="I33" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI34</f>
         <v>3.5</v>
       </c>
-      <c r="J33" s="33" t="n">
+      <c r="J33" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN34</f>
         <v>9533.1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="41" t="n">
+      <c r="B34" s="143" t="n">
         <f aca="false">1/(15/1000)</f>
         <v>66.6666666666667</v>
       </c>
-      <c r="C34" s="28" t="n">
+      <c r="C34" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D35/$B34</f>
         <v>0.3243</v>
       </c>
-      <c r="D34" s="30" t="n">
+      <c r="D34" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J35/$B34</f>
         <v>0.42795</v>
       </c>
-      <c r="E34" s="28" t="n">
+      <c r="E34" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P35/$B34</f>
         <v>0.41475</v>
       </c>
-      <c r="F34" s="30" t="n">
+      <c r="F34" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V35/$B34</f>
         <v>1.2471</v>
       </c>
-      <c r="G34" s="28" t="n">
+      <c r="G34" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB35/$B34</f>
         <v>1.6578</v>
       </c>
-      <c r="H34" s="33" t="n">
+      <c r="H34" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH35/$B34</f>
         <v>0.3885</v>
       </c>
-      <c r="I34" s="33" t="n">
+      <c r="I34" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI35/$B34</f>
         <v>0.4995</v>
       </c>
-      <c r="J34" s="33" t="n">
+      <c r="J34" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN35/$B34</f>
         <v>5.055</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="40" t="n">
+      <c r="B35" s="142" t="n">
         <f aca="false">1/(50/1000)</f>
         <v>20</v>
       </c>
-      <c r="C35" s="28" t="n">
+      <c r="C35" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D36/$B35</f>
         <v>3.448</v>
       </c>
-      <c r="D35" s="30" t="n">
+      <c r="D35" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J36/$B35</f>
         <v>2.3325</v>
       </c>
-      <c r="E35" s="28" t="n">
+      <c r="E35" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P36/$B35</f>
         <v>2.314</v>
       </c>
-      <c r="F35" s="30" t="n">
+      <c r="F35" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V36/$B35</f>
         <v>2.315</v>
       </c>
-      <c r="G35" s="28" t="n">
+      <c r="G35" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB36/$B35</f>
         <v>4.354</v>
       </c>
-      <c r="H35" s="33" t="n">
+      <c r="H35" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH36/$B35</f>
         <v>27.03</v>
       </c>
-      <c r="I35" s="33" t="n">
+      <c r="I35" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI36/$B35</f>
         <v>1.245</v>
       </c>
-      <c r="J35" s="33" t="n">
+      <c r="J35" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN36/$B35</f>
         <v>143.96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="27" t="n">
+      <c r="B36" s="136" t="n">
         <v>1.994</v>
       </c>
-      <c r="C36" s="28" t="n">
+      <c r="C36" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D37/$B36</f>
         <v>163.595787362086</v>
       </c>
-      <c r="D36" s="30" t="n">
+      <c r="D36" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J37/$B36</f>
         <v>49.8896690070211</v>
       </c>
-      <c r="E36" s="28" t="n">
+      <c r="E36" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P37/$B36</f>
         <v>42.7231695085256</v>
       </c>
-      <c r="F36" s="30" t="n">
+      <c r="F36" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V37/$B36</f>
         <v>159.894684052156</v>
       </c>
-      <c r="G36" s="28" t="n">
+      <c r="G36" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB37/$B36</f>
         <v>151.158475426279</v>
       </c>
-      <c r="H36" s="33" t="n">
+      <c r="H36" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH37/$B36</f>
         <v>727.78335005015</v>
       </c>
-      <c r="I36" s="33" t="n">
+      <c r="I36" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI37/$B36</f>
         <v>371.213640922768</v>
       </c>
-      <c r="J36" s="33" t="n">
+      <c r="J36" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN37/$B36</f>
         <v>17418.5055165497</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="27" t="n">
+      <c r="B37" s="136" t="n">
         <v>1.974</v>
       </c>
-      <c r="C37" s="28" t="n">
+      <c r="C37" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D38/$B37</f>
         <v>21.9047619047619</v>
       </c>
-      <c r="D37" s="30" t="n">
+      <c r="D37" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J38/$B37</f>
         <v>16.8693009118541</v>
       </c>
-      <c r="E37" s="28" t="n">
+      <c r="E37" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P38/$B37</f>
         <v>14.5845997973658</v>
       </c>
-      <c r="F37" s="30" t="n">
+      <c r="F37" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V38/$B37</f>
         <v>174.083080040527</v>
       </c>
-      <c r="G37" s="28" t="n">
+      <c r="G37" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB38/$B37</f>
         <v>185.050658561297</v>
       </c>
-      <c r="H37" s="33" t="n">
+      <c r="H37" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH38/$B37</f>
         <v>1375.02532928065</v>
       </c>
-      <c r="I37" s="33" t="n">
+      <c r="I37" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI38/$B37</f>
         <v>1324.31610942249</v>
       </c>
-      <c r="J37" s="33" t="n">
+      <c r="J37" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN38/$B37</f>
         <v>60691.5906788247</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="130" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="27" t="n">
+      <c r="B38" s="136" t="n">
         <v>2.001</v>
       </c>
-      <c r="C38" s="28" t="n">
+      <c r="C38" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D39/$B38</f>
         <v>184.812593703148</v>
       </c>
-      <c r="D38" s="30" t="n">
+      <c r="D38" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J39/$B38</f>
         <v>19.8500749625187</v>
       </c>
-      <c r="E38" s="28" t="n">
+      <c r="E38" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P39/$B38</f>
         <v>16.3468265867066</v>
       </c>
-      <c r="F38" s="30" t="n">
+      <c r="F38" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V39/$B38</f>
         <v>69.4502748625687</v>
       </c>
-      <c r="G38" s="28" t="n">
+      <c r="G38" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB39/$B38</f>
         <v>48.5407296351824</v>
       </c>
-      <c r="H38" s="33" t="n">
+      <c r="H38" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH39/$B38</f>
         <v>900.949525237381</v>
       </c>
-      <c r="I38" s="33" t="n">
+      <c r="I38" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI39/$B38</f>
         <v>230.484757621189</v>
       </c>
-      <c r="J38" s="33" t="n">
+      <c r="J38" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN39/$B38</f>
         <v>70927.0364817591</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="130" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="27" t="n">
+      <c r="B39" s="136" t="n">
         <v>1.618</v>
       </c>
-      <c r="C39" s="28" t="n">
+      <c r="C39" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D40/$B39</f>
         <v>10.7292954264524</v>
       </c>
-      <c r="D39" s="30" t="n">
+      <c r="D39" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J40/$B39</f>
         <v>7.60815822002472</v>
       </c>
-      <c r="E39" s="28" t="n">
+      <c r="E39" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P40/$B39</f>
         <v>7.13226205191594</v>
       </c>
-      <c r="F39" s="30" t="n">
+      <c r="F39" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V40/$B39</f>
         <v>88.1705809641533</v>
       </c>
-      <c r="G39" s="28" t="n">
+      <c r="G39" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB40/$B39</f>
         <v>47.2064276885043</v>
       </c>
-      <c r="H39" s="33" t="n">
+      <c r="H39" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH40/$B39</f>
         <v>1109.88875154512</v>
       </c>
-      <c r="I39" s="33" t="n">
+      <c r="I39" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI40/$B39</f>
         <v>1118.85043263288</v>
       </c>
-      <c r="J39" s="33" t="n">
+      <c r="J39" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN40/$B39</f>
         <v>41327.1940667491</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="27" t="n">
+      <c r="B40" s="136" t="n">
         <v>1.732</v>
       </c>
-      <c r="C40" s="28" t="n">
+      <c r="C40" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D41/$B40</f>
         <v>7.0554272517321</v>
       </c>
-      <c r="D40" s="30" t="n">
+      <c r="D40" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J41/$B40</f>
         <v>5.6986143187067</v>
       </c>
-      <c r="E40" s="28" t="n">
+      <c r="E40" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P41/$B40</f>
         <v>5.66974595842956</v>
       </c>
-      <c r="F40" s="30" t="n">
+      <c r="F40" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V41/$B40</f>
         <v>59.1339491916859</v>
       </c>
-      <c r="G40" s="28" t="n">
+      <c r="G40" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB41/$B40</f>
         <v>28.1177829099307</v>
       </c>
-      <c r="H40" s="33" t="n">
+      <c r="H40" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH41/$B40</f>
         <v>381.062355658199</v>
       </c>
-      <c r="I40" s="33" t="n">
+      <c r="I40" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI41/$B40</f>
         <v>213.799076212471</v>
       </c>
-      <c r="J40" s="33" t="n">
+      <c r="J40" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN41/$B40</f>
         <v>8185.8545034642</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="28" t="n">
+      <c r="B41" s="141" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D42</f>
         <v>8.95</v>
       </c>
-      <c r="D41" s="30" t="n">
+      <c r="D41" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J42</f>
         <v>3.15</v>
       </c>
-      <c r="E41" s="28" t="n">
+      <c r="E41" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P42</f>
         <v>2.84</v>
       </c>
-      <c r="F41" s="30" t="n">
+      <c r="F41" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V42</f>
         <v>20.01</v>
       </c>
-      <c r="G41" s="28" t="n">
+      <c r="G41" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB42</f>
         <v>10.65</v>
       </c>
-      <c r="H41" s="33" t="n">
+      <c r="H41" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH42</f>
         <v>628.2</v>
       </c>
-      <c r="I41" s="33" t="n">
+      <c r="I41" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI42</f>
         <v>197.3</v>
       </c>
-      <c r="J41" s="33" t="n">
+      <c r="J41" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN42</f>
         <v>19786.3</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="27" t="n">
+      <c r="B42" s="136" t="n">
         <v>2.208</v>
       </c>
-      <c r="C42" s="28" t="n">
+      <c r="C42" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D43/$B42</f>
         <v>39.7599637681159</v>
       </c>
-      <c r="D42" s="30" t="n">
+      <c r="D42" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J43/$B42</f>
         <v>10.8152173913043</v>
       </c>
-      <c r="E42" s="28" t="n">
+      <c r="E42" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P43/$B42</f>
         <v>9.71014492753623</v>
       </c>
-      <c r="F42" s="30" t="n">
+      <c r="F42" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V43/$B42</f>
         <v>74.9728260869565</v>
       </c>
-      <c r="G42" s="28" t="n">
+      <c r="G42" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB43/$B42</f>
         <v>44.5516304347826</v>
       </c>
-      <c r="H42" s="33" t="n">
+      <c r="H42" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH43/$B42</f>
         <v>2538.58695652174</v>
       </c>
-      <c r="I42" s="33" t="n">
+      <c r="I42" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI43/$B42</f>
         <v>706.204710144928</v>
       </c>
-      <c r="J42" s="33" t="n">
+      <c r="J42" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN43/$B42</f>
         <v>81906.9746376812</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="130" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="27" t="n">
+      <c r="B43" s="136" t="n">
         <v>1.1096</v>
       </c>
-      <c r="C43" s="28" t="n">
+      <c r="C43" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D44/$B43</f>
         <v>5.65068493150685</v>
       </c>
-      <c r="D43" s="30" t="n">
+      <c r="D43" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J44/$B43</f>
         <v>4.20872386445566</v>
       </c>
-      <c r="E43" s="28" t="n">
+      <c r="E43" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P44/$B43</f>
         <v>4.14563806777217</v>
       </c>
-      <c r="F43" s="30" t="n">
+      <c r="F43" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V44/$B43</f>
         <v>48.3687815428984</v>
       </c>
-      <c r="G43" s="28" t="n">
+      <c r="G43" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB44/$B43</f>
         <v>19.6106705118962</v>
       </c>
-      <c r="H43" s="33" t="n">
+      <c r="H43" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH44/$B43</f>
         <v>520.63806777217</v>
       </c>
-      <c r="I43" s="33" t="n">
+      <c r="I43" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI44/$B43</f>
         <v>570.385724585436</v>
       </c>
-      <c r="J43" s="33" t="n">
+      <c r="J43" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN44/$B43</f>
         <v>16206.4708002884</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="27" t="n">
+      <c r="B44" s="136" t="n">
         <v>2.2805</v>
       </c>
-      <c r="C44" s="28" t="n">
+      <c r="C44" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D45/$B44</f>
         <v>3.68778776584082</v>
       </c>
-      <c r="D44" s="30" t="n">
+      <c r="D44" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J45/$B44</f>
         <v>5.97675948256961</v>
       </c>
-      <c r="E44" s="28" t="n">
+      <c r="E44" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P45/$B44</f>
         <v>5.48563911422934</v>
       </c>
-      <c r="F44" s="30" t="n">
+      <c r="F44" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V45/$B44</f>
         <v>28.9015566761675</v>
       </c>
-      <c r="G44" s="28" t="n">
+      <c r="G44" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB45/$B44</f>
         <v>103.100197325148</v>
       </c>
-      <c r="H44" s="33" t="n">
+      <c r="H44" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH45/$B44</f>
         <v>1618.6362639772</v>
       </c>
-      <c r="I44" s="33" t="n">
+      <c r="I44" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI45/$B44</f>
         <v>693.049769787327</v>
       </c>
-      <c r="J44" s="33" t="n">
+      <c r="J44" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN45/$B44</f>
         <v>18229.4233720675</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="27" t="n">
+      <c r="B45" s="136" t="n">
         <v>1.477</v>
       </c>
-      <c r="C45" s="28" t="n">
+      <c r="C45" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!D46/$B45</f>
         <v>2.01083276912661</v>
       </c>
-      <c r="D45" s="30" t="n">
+      <c r="D45" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!J46/$B45</f>
         <v>18.1922816519973</v>
       </c>
-      <c r="E45" s="28" t="n">
+      <c r="E45" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!P46/$B45</f>
         <v>16.2423832092079</v>
       </c>
-      <c r="F45" s="30" t="n">
+      <c r="F45" s="138" t="n">
         <f aca="false">'Results - Retail Weight'!V46/$B45</f>
         <v>90.0947867298578</v>
       </c>
-      <c r="G45" s="28" t="n">
+      <c r="G45" s="137" t="n">
         <f aca="false">'Results - Retail Weight'!AB46/$B45</f>
         <v>153.838862559242</v>
       </c>
-      <c r="H45" s="33" t="n">
+      <c r="H45" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AH46/$B45</f>
         <v>2380.09478672986</v>
       </c>
-      <c r="I45" s="33" t="n">
+      <c r="I45" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AI46/$B45</f>
         <v>817.738659444821</v>
       </c>
-      <c r="J45" s="33" t="n">
+      <c r="J45" s="139" t="n">
         <f aca="false">'Results - Retail Weight'!AN46/$B45</f>
         <v>86160.4603926879</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="42"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="44"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="46"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47" t="n">
-        <f aca="false">MAX(D12:D13,D15,D17)</f>
-        <v>1.975</v>
-      </c>
-      <c r="E48" s="47" t="n">
-        <f aca="false">MAX(E12:E13,E15,E17)</f>
-        <v>1.9625</v>
-      </c>
-      <c r="F48" s="47" t="n">
-        <f aca="false">MAX(F12:F13,F15,F17)</f>
-        <v>10.3082671648762</v>
-      </c>
-      <c r="G48" s="47" t="n">
-        <f aca="false">MAX(G12:G13,G15,G17)</f>
-        <v>7.97758056982718</v>
-      </c>
-      <c r="H48" s="47"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="46"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="51" t="n">
-        <f aca="false">MAX(D12:D15,D17)</f>
-        <v>1.975</v>
-      </c>
-      <c r="E49" s="51" t="n">
-        <f aca="false">MAX(E12:E15,E17)</f>
-        <v>1.9625</v>
-      </c>
-      <c r="F49" s="51" t="n">
-        <f aca="false">MAX(F12:F15,F17)</f>
-        <v>27.6484996938151</v>
-      </c>
-      <c r="G49" s="51" t="n">
-        <f aca="false">MAX(G12:G15,G17)</f>
-        <v>11.7268830373546</v>
-      </c>
-      <c r="H49" s="51"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A50:D51"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>